<commit_message>
Modification pour question 4 et 8
</commit_message>
<xml_diff>
--- a/doc/LBS-stories-LP2.xlsx
+++ b/doc/LBS-stories-LP2.xlsx
@@ -92,9 +92,6 @@
     <t>Obtenir la description d'un sandwich</t>
   </si>
   <si>
-    <t>sandwichs/{id}?fields=description</t>
-  </si>
-  <si>
     <t>sandwich par catégorie</t>
   </si>
   <si>
@@ -128,9 +125,6 @@
     <t>Obtenir la description détaillée d'un sandwich avec les tailles, prix et catégories du sandwich sous forme de liste imbriquée</t>
   </si>
   <si>
-    <t>sandwichs/{id}</t>
-  </si>
-  <si>
     <t>créer une commande</t>
   </si>
   <si>
@@ -276,6 +270,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>sandwichs/{id}[?details=0]</t>
+  </si>
+  <si>
+    <t>sandwichs/{id}?details=1</t>
   </si>
 </sst>
 </file>
@@ -825,7 +825,7 @@
   <dimension ref="A1:V1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1027,7 +1027,7 @@
         <v>12</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1067,7 +1067,7 @@
         <v>15</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -1107,7 +1107,7 @@
         <v>18</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -1144,10 +1144,10 @@
         <v>11</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -1172,10 +1172,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="E11" s="9">
         <v>3</v>
@@ -1184,10 +1184,10 @@
         <v>11</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -1212,10 +1212,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="E12" s="9">
         <v>3</v>
@@ -1224,10 +1224,10 @@
         <v>11</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1252,10 +1252,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="10" t="s">
         <v>28</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="E13" s="9">
         <v>3</v>
@@ -1264,10 +1264,10 @@
         <v>11</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1292,10 +1292,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>32</v>
       </c>
       <c r="E14" s="9">
         <v>3</v>
@@ -1304,10 +1304,10 @@
         <v>11</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1332,22 +1332,22 @@
         <v>1</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E15" s="9">
         <v>4</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1372,19 +1372,19 @@
         <v>1</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" s="9">
         <v>6</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="2"/>
@@ -1410,19 +1410,19 @@
         <v>1</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E17" s="9">
         <v>4</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="2"/>
@@ -1448,19 +1448,19 @@
         <v>1</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E18" s="9">
         <v>3</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="2"/>
@@ -1486,10 +1486,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E19" s="9">
         <v>2</v>
@@ -1498,7 +1498,7 @@
         <v>11</v>
       </c>
       <c r="G19" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="2"/>
@@ -1524,19 +1524,19 @@
         <v>2</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E20" s="9">
         <v>3</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="2"/>
@@ -1562,19 +1562,19 @@
         <v>2</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E21" s="9">
         <v>3</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="2"/>
@@ -1600,10 +1600,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E22" s="9">
         <v>4</v>
@@ -1612,7 +1612,7 @@
         <v>11</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="2"/>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B23" s="13"/>
       <c r="C23" s="14"/>
@@ -1702,10 +1702,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E25" s="9">
         <v>3</v>
@@ -1736,10 +1736,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E26" s="9">
         <v>3</v>
@@ -1770,10 +1770,10 @@
         <v>1</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E27" s="9">
         <v>3</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="17"/>
@@ -1868,10 +1868,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D30" s="19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E30" s="9">
         <v>5</v>
@@ -1902,10 +1902,10 @@
         <v>1</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E31" s="9">
         <v>5</v>
@@ -1936,10 +1936,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E32" s="9">
         <v>6</v>
@@ -1970,10 +1970,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E33" s="9">
         <v>4</v>
@@ -1998,7 +1998,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B34" s="16"/>
       <c r="C34" s="17"/>
@@ -2068,10 +2068,10 @@
         <v>1</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E36" s="9">
         <v>3</v>
@@ -2102,10 +2102,10 @@
         <v>1</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E37" s="20">
         <v>6</v>
@@ -2136,10 +2136,10 @@
         <v>1</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E38" s="20">
         <v>3</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D40" s="24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E40">
         <f>SUM(E7:E38)</f>

</xml_diff>

<commit_message>
Updating error and success messages and remove sandwich to commande
</commit_message>
<xml_diff>
--- a/doc/LBS-stories-LP2.xlsx
+++ b/doc/LBS-stories-LP2.xlsx
@@ -14,6 +14,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
   <si>
     <t xml:space="preserve">USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -589,21 +590,21 @@
   <dimension ref="A1:V65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3775510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.5918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.75"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="22" min="9" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.9183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="33.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="22" min="9" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="18.3571428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1268,7 +1269,9 @@
       <c r="G19" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -1306,7 +1309,9 @@
       <c r="G20" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>

</xml_diff>

<commit_message>
Correction date, début carte fidel castro
</commit_message>
<xml_diff>
--- a/doc/LBS-stories-LP2.xlsx
+++ b/doc/LBS-stories-LP2.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="89">
   <si>
     <t>USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -290,6 +290,12 @@
   </si>
   <si>
     <t>card[?token=]</t>
+  </si>
+  <si>
+    <t>card/checkout[?token=]</t>
+  </si>
+  <si>
+    <t>card</t>
   </si>
 </sst>
 </file>
@@ -346,7 +352,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +363,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF0DB4F"/>
         <bgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -387,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -457,6 +469,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -846,8 +867,8 @@
   </sheetPr>
   <dimension ref="A1:V1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -974,7 +995,7 @@
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
@@ -1014,7 +1035,7 @@
       <c r="I6" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -1054,7 +1075,7 @@
         <v>13</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
+      <c r="J7" s="2"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
@@ -1094,7 +1115,7 @@
         <v>13</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="J8" s="2"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1134,7 +1155,7 @@
         <v>13</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
+      <c r="J9" s="2"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
@@ -1174,7 +1195,7 @@
         <v>13</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="J10" s="2"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -1214,7 +1235,7 @@
         <v>13</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
+      <c r="J11" s="28"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -1254,7 +1275,7 @@
         <v>13</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="J12" s="28"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -1294,7 +1315,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="J13" s="28"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -1334,7 +1355,7 @@
         <v>13</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="J14" s="28"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -1374,7 +1395,7 @@
         <v>13</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="J15" s="28"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -1414,7 +1435,7 @@
         <v>13</v>
       </c>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="J16" s="28"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -1454,7 +1475,7 @@
         <v>13</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
+      <c r="J17" s="28"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -1490,9 +1511,9 @@
       <c r="G18" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="27"/>
       <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="J18" s="28"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -1532,7 +1553,7 @@
         <v>13</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
+      <c r="J19" s="28"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -1572,7 +1593,7 @@
         <v>13</v>
       </c>
       <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="J20" s="28"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -1608,9 +1629,9 @@
       <c r="G21" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="27"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
+      <c r="J21" s="28"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -1646,9 +1667,9 @@
       <c r="G22" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="27"/>
       <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="J22" s="28"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -1674,7 +1695,7 @@
       <c r="G23" s="14"/>
       <c r="H23" s="16"/>
       <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="J23" s="29"/>
       <c r="K23" s="17"/>
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
@@ -1712,7 +1733,7 @@
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="J24" s="28"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -1744,9 +1765,9 @@
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
-      <c r="H25" s="2"/>
+      <c r="H25" s="27"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="J25" s="28"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -1778,9 +1799,9 @@
       </c>
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
-      <c r="H26" s="2"/>
+      <c r="H26" s="27"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="J26" s="28"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -1812,9 +1833,9 @@
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
-      <c r="H27" s="2"/>
+      <c r="H27" s="27"/>
       <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="J27" s="28"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -1840,7 +1861,7 @@
       <c r="G28" s="18"/>
       <c r="H28" s="16"/>
       <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
+      <c r="J28" s="29"/>
       <c r="K28" s="17"/>
       <c r="L28" s="17"/>
       <c r="M28" s="17"/>
@@ -1878,7 +1899,7 @@
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
+      <c r="J29" s="28"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -1918,7 +1939,7 @@
         <v>13</v>
       </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="J30" s="28"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -1949,14 +1970,14 @@
         <v>5</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="H31" s="2"/>
+      <c r="H31" s="27"/>
       <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="J31" s="28"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -1986,11 +2007,15 @@
       <c r="E32" s="10">
         <v>6</v>
       </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="2"/>
+      <c r="F32" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" s="27"/>
       <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="J32" s="28"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -2020,11 +2045,15 @@
       <c r="E33" s="10">
         <v>4</v>
       </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="2"/>
+      <c r="F33" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H33" s="27"/>
       <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
+      <c r="J33" s="28"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -2050,7 +2079,7 @@
       <c r="G34" s="18"/>
       <c r="H34" s="16"/>
       <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
+      <c r="J34" s="29"/>
       <c r="K34" s="17"/>
       <c r="L34" s="17"/>
       <c r="M34" s="17"/>
@@ -2088,7 +2117,7 @@
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
+      <c r="J35" s="28"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -2128,7 +2157,7 @@
         <v>13</v>
       </c>
       <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
+      <c r="J36" s="28"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -2164,9 +2193,9 @@
       <c r="G37" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="H37" s="2"/>
+      <c r="H37" s="27"/>
       <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
+      <c r="J37" s="28"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -2202,9 +2231,9 @@
       <c r="G38" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="H38" s="2"/>
+      <c r="H38" s="27"/>
       <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
+      <c r="J38" s="28"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>

</xml_diff>

<commit_message>
Création carte et récupération carte
</commit_message>
<xml_diff>
--- a/doc/LBS-stories-LP2.xlsx
+++ b/doc/LBS-stories-LP2.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
   <si>
     <t>USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -70,9 +70,6 @@
     <t>categories/{id}</t>
   </si>
   <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>collection de catégories</t>
   </si>
   <si>
@@ -292,10 +289,13 @@
     <t>card[?token=]</t>
   </si>
   <si>
-    <t>card/checkout[?token=]</t>
-  </si>
-  <si>
-    <t>card</t>
+    <t>REALISE</t>
+  </si>
+  <si>
+    <t>card/create</t>
+  </si>
+  <si>
+    <t>card/{id}/checkout[?token=]</t>
   </si>
 </sst>
 </file>
@@ -352,7 +352,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +368,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -399,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -480,6 +486,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,8 +878,8 @@
   </sheetPr>
   <dimension ref="A1:V1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -880,7 +891,7 @@
     <col min="5" max="5" width="11.28515625"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
     <col min="7" max="7" width="33.28515625"/>
-    <col min="8" max="8" width="9.28515625" style="1"/>
+    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
     <col min="9" max="22" width="9.28515625"/>
     <col min="23" max="1025" width="18.28515625"/>
   </cols>
@@ -1031,9 +1042,11 @@
       <c r="G6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="26" t="s">
+        <v>86</v>
+      </c>
       <c r="I6" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="3"/>
@@ -1071,10 +1084,8 @@
       <c r="G7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="3"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="32"/>
       <c r="J7" s="2"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -1097,10 +1108,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>15</v>
       </c>
       <c r="E8" s="10">
         <v>2</v>
@@ -1109,12 +1120,10 @@
         <v>11</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="H8" s="31"/>
+      <c r="I8" s="32"/>
       <c r="J8" s="2"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -1137,10 +1146,10 @@
         <v>1</v>
       </c>
       <c r="C9" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="E9" s="10">
         <v>2</v>
@@ -1149,12 +1158,10 @@
         <v>11</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I9" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="H9" s="31"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="2"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -1177,10 +1184,10 @@
         <v>1</v>
       </c>
       <c r="C10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="E10" s="10">
         <v>2</v>
@@ -1189,12 +1196,10 @@
         <v>11</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I10" s="3"/>
+        <v>21</v>
+      </c>
+      <c r="H10" s="31"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="2"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1217,10 +1222,10 @@
         <v>1</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="E11" s="10">
         <v>3</v>
@@ -1229,12 +1234,10 @@
         <v>11</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="H11" s="31"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="28"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -1257,10 +1260,10 @@
         <v>1</v>
       </c>
       <c r="C12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="E12" s="10">
         <v>3</v>
@@ -1269,12 +1272,10 @@
         <v>11</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I12" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="H12" s="31"/>
+      <c r="I12" s="32"/>
       <c r="J12" s="28"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -1297,10 +1298,10 @@
         <v>1</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>29</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>30</v>
       </c>
       <c r="E13" s="10">
         <v>3</v>
@@ -1309,12 +1310,10 @@
         <v>11</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="H13" s="31"/>
+      <c r="I13" s="32"/>
       <c r="J13" s="28"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1337,10 +1336,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="E14" s="10">
         <v>3</v>
@@ -1349,12 +1348,10 @@
         <v>11</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="H14" s="31"/>
+      <c r="I14" s="32"/>
       <c r="J14" s="28"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1377,24 +1374,22 @@
         <v>1</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="E15" s="10">
         <v>4</v>
       </c>
       <c r="F15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="3"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="32"/>
       <c r="J15" s="28"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
@@ -1417,24 +1412,22 @@
         <v>1</v>
       </c>
       <c r="C16" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="E16" s="10">
         <v>6</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="H16" s="31"/>
+      <c r="I16" s="32"/>
       <c r="J16" s="28"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1457,24 +1450,22 @@
         <v>1</v>
       </c>
       <c r="C17" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="E17" s="10">
         <v>4</v>
       </c>
       <c r="F17" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G17" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="3"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="32"/>
       <c r="J17" s="28"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
@@ -1497,22 +1488,22 @@
         <v>1</v>
       </c>
       <c r="C18" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="11" t="s">
         <v>46</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="E18" s="10">
         <v>3</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="27"/>
-      <c r="I18" s="3"/>
+      <c r="I18" s="32"/>
       <c r="J18" s="28"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
@@ -1535,10 +1526,10 @@
         <v>1</v>
       </c>
       <c r="C19" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>50</v>
       </c>
       <c r="E19" s="10">
         <v>2</v>
@@ -1547,12 +1538,10 @@
         <v>11</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="H19" s="31"/>
+      <c r="I19" s="32"/>
       <c r="J19" s="28"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
@@ -1575,24 +1564,22 @@
         <v>2</v>
       </c>
       <c r="C20" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="11" t="s">
         <v>51</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="E20" s="10">
         <v>3</v>
       </c>
       <c r="F20" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I20" s="3"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="32"/>
       <c r="J20" s="28"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -1615,22 +1602,22 @@
         <v>2</v>
       </c>
       <c r="C21" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="E21" s="10">
         <v>3</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H21" s="27"/>
-      <c r="I21" s="3"/>
+      <c r="I21" s="32"/>
       <c r="J21" s="28"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
@@ -1653,10 +1640,10 @@
         <v>2</v>
       </c>
       <c r="C22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>58</v>
       </c>
       <c r="E22" s="10">
         <v>4</v>
@@ -1665,10 +1652,10 @@
         <v>11</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H22" s="27"/>
-      <c r="I22" s="3"/>
+      <c r="I22" s="32"/>
       <c r="J22" s="28"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
@@ -1685,7 +1672,7 @@
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -1755,10 +1742,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>62</v>
       </c>
       <c r="E25" s="10">
         <v>3</v>
@@ -1766,7 +1753,7 @@
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
       <c r="H25" s="27"/>
-      <c r="I25" s="3"/>
+      <c r="I25" s="32"/>
       <c r="J25" s="28"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
@@ -1789,10 +1776,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>64</v>
       </c>
       <c r="E26" s="10">
         <v>3</v>
@@ -1800,7 +1787,7 @@
       <c r="F26" s="12"/>
       <c r="G26" s="12"/>
       <c r="H26" s="27"/>
-      <c r="I26" s="3"/>
+      <c r="I26" s="32"/>
       <c r="J26" s="28"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
@@ -1823,10 +1810,10 @@
         <v>1</v>
       </c>
       <c r="C27" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="E27" s="10">
         <v>3</v>
@@ -1834,7 +1821,7 @@
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="27"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="32"/>
       <c r="J27" s="28"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
@@ -1851,7 +1838,7 @@
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B28" s="18"/>
       <c r="C28" s="19"/>
@@ -1921,24 +1908,22 @@
         <v>1</v>
       </c>
       <c r="C30" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="21" t="s">
         <v>68</v>
-      </c>
-      <c r="D30" s="21" t="s">
-        <v>69</v>
       </c>
       <c r="E30" s="10">
         <v>5</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I30" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="H30" s="31"/>
+      <c r="I30" s="30"/>
       <c r="J30" s="28"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -1961,22 +1946,22 @@
         <v>1</v>
       </c>
       <c r="C31" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>72</v>
       </c>
       <c r="E31" s="10">
         <v>5</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="H31" s="27"/>
-      <c r="I31" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="H31" s="31"/>
+      <c r="I31" s="32"/>
       <c r="J31" s="28"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
@@ -1999,22 +1984,22 @@
         <v>1</v>
       </c>
       <c r="C32" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="E32" s="10">
         <v>6</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H32" s="27"/>
-      <c r="I32" s="3"/>
+      <c r="I32" s="32"/>
       <c r="J32" s="28"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
@@ -2037,22 +2022,22 @@
         <v>3</v>
       </c>
       <c r="C33" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="E33" s="10">
         <v>4</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="H33" s="27"/>
-      <c r="I33" s="3"/>
+        <v>87</v>
+      </c>
+      <c r="H33" s="31"/>
+      <c r="I33" s="32"/>
       <c r="J33" s="28"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
@@ -2069,7 +2054,7 @@
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="18"/>
       <c r="C34" s="19"/>
@@ -2139,24 +2124,22 @@
         <v>1</v>
       </c>
       <c r="C36" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="21" t="s">
         <v>78</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>79</v>
       </c>
       <c r="E36" s="10">
         <v>3</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="H36" s="31"/>
+      <c r="I36" s="30"/>
       <c r="J36" s="28"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
@@ -2179,22 +2162,22 @@
         <v>1</v>
       </c>
       <c r="C37" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D37" s="24" t="s">
         <v>80</v>
-      </c>
-      <c r="D37" s="24" t="s">
-        <v>81</v>
       </c>
       <c r="E37" s="22">
         <v>6</v>
       </c>
       <c r="F37" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G37" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H37" s="27"/>
-      <c r="I37" s="3"/>
+      <c r="I37" s="32"/>
       <c r="J37" s="28"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
@@ -2217,22 +2200,22 @@
         <v>1</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E38" s="22">
         <v>3</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H38" s="27"/>
-      <c r="I38" s="3"/>
+      <c r="I38" s="32"/>
       <c r="J38" s="28"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
@@ -2249,7 +2232,7 @@
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D40" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E40">
         <f>SUM(E7:E38)</f>

</xml_diff>

<commit_message>
Mise a jour de l'ajout de sandwich a la commande, de la modif de sandwich dans la commande et de l'affichage d'une commande
</commit_message>
<xml_diff>
--- a/doc/LBS-stories-LP2.xlsx
+++ b/doc/LBS-stories-LP2.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="Print_Area_0" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="Print_Area_0_0" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -428,7 +429,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -493,14 +494,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -521,7 +514,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -641,20 +634,21 @@
   <dimension ref="A1:V65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.2397959183674"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="9" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.7040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="22" min="9" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -999,7 +993,7 @@
       </c>
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
-      <c r="J11" s="16"/>
+      <c r="J11" s="2"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
@@ -1037,7 +1031,7 @@
       </c>
       <c r="H12" s="14"/>
       <c r="I12" s="15"/>
-      <c r="J12" s="16"/>
+      <c r="J12" s="2"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -1075,7 +1069,7 @@
       </c>
       <c r="H13" s="14"/>
       <c r="I13" s="15"/>
-      <c r="J13" s="16"/>
+      <c r="J13" s="2"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -1113,7 +1107,7 @@
       </c>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="16"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -1151,7 +1145,7 @@
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="15"/>
-      <c r="J15" s="16"/>
+      <c r="J15" s="2"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
@@ -1189,7 +1183,7 @@
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="15"/>
-      <c r="J16" s="16"/>
+      <c r="J16" s="2"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -1227,7 +1221,7 @@
       </c>
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
-      <c r="J17" s="16"/>
+      <c r="J17" s="2"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
@@ -1265,7 +1259,7 @@
       </c>
       <c r="H18" s="14"/>
       <c r="I18" s="15"/>
-      <c r="J18" s="16"/>
+      <c r="J18" s="2"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
@@ -1303,7 +1297,7 @@
       </c>
       <c r="H19" s="14"/>
       <c r="I19" s="15"/>
-      <c r="J19" s="16"/>
+      <c r="J19" s="2"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
@@ -1341,7 +1335,7 @@
       </c>
       <c r="H20" s="14"/>
       <c r="I20" s="15"/>
-      <c r="J20" s="16"/>
+      <c r="J20" s="2"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
@@ -1377,9 +1371,9 @@
       <c r="G21" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H21" s="17"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="15"/>
-      <c r="J21" s="16"/>
+      <c r="J21" s="2"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
@@ -1393,7 +1387,7 @@
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="n">
         <v>16</v>
       </c>
@@ -1415,9 +1409,9 @@
       <c r="G22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="17"/>
+      <c r="H22" s="14"/>
       <c r="I22" s="15"/>
-      <c r="J22" s="16"/>
+      <c r="J22" s="2"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
@@ -1432,30 +1426,30 @@
       <c r="V22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
-      <c r="T23" s="22"/>
-      <c r="U23" s="22"/>
-      <c r="V23" s="22"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="20"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
@@ -1481,7 +1475,7 @@
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="3"/>
-      <c r="J24" s="16"/>
+      <c r="J24" s="2"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
@@ -1513,9 +1507,9 @@
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
-      <c r="H25" s="17"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="15"/>
-      <c r="J25" s="16"/>
+      <c r="J25" s="2"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -1547,9 +1541,9 @@
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
-      <c r="H26" s="17"/>
+      <c r="H26" s="21"/>
       <c r="I26" s="15"/>
-      <c r="J26" s="16"/>
+      <c r="J26" s="2"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -1581,9 +1575,9 @@
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
-      <c r="H27" s="17"/>
+      <c r="H27" s="21"/>
       <c r="I27" s="15"/>
-      <c r="J27" s="16"/>
+      <c r="J27" s="2"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -1601,27 +1595,27 @@
       <c r="A28" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="22"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="22"/>
-      <c r="S28" s="22"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="22"/>
-      <c r="V28" s="22"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="20"/>
+      <c r="U28" s="20"/>
+      <c r="V28" s="20"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
@@ -1647,7 +1641,7 @@
       </c>
       <c r="H29" s="2"/>
       <c r="I29" s="3"/>
-      <c r="J29" s="16"/>
+      <c r="J29" s="2"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
@@ -1668,10 +1662,10 @@
       <c r="B30" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="25" t="s">
         <v>70</v>
       </c>
       <c r="E30" s="11" t="n">
@@ -1684,8 +1678,8 @@
         <v>71</v>
       </c>
       <c r="H30" s="14"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="16"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="2"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
@@ -1723,7 +1717,7 @@
       </c>
       <c r="H31" s="14"/>
       <c r="I31" s="15"/>
-      <c r="J31" s="16"/>
+      <c r="J31" s="2"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -1759,9 +1753,9 @@
       <c r="G32" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="H32" s="17"/>
+      <c r="H32" s="21"/>
       <c r="I32" s="15"/>
-      <c r="J32" s="16"/>
+      <c r="J32" s="2"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -1799,7 +1793,7 @@
       </c>
       <c r="H33" s="14"/>
       <c r="I33" s="15"/>
-      <c r="J33" s="16"/>
+      <c r="J33" s="2"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -1817,27 +1811,27 @@
       <c r="A34" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="22"/>
-      <c r="S34" s="22"/>
-      <c r="T34" s="22"/>
-      <c r="U34" s="22"/>
-      <c r="V34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="20"/>
+      <c r="S34" s="20"/>
+      <c r="T34" s="20"/>
+      <c r="U34" s="20"/>
+      <c r="V34" s="20"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="9" t="s">
@@ -1863,7 +1857,7 @@
       </c>
       <c r="H35" s="2"/>
       <c r="I35" s="3"/>
-      <c r="J35" s="16"/>
+      <c r="J35" s="2"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
@@ -1884,10 +1878,10 @@
       <c r="B36" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="25" t="s">
         <v>83</v>
       </c>
       <c r="E36" s="11" t="n">
@@ -1900,8 +1894,8 @@
         <v>84</v>
       </c>
       <c r="H36" s="14"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="16"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="2"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
@@ -1916,30 +1910,30 @@
       <c r="V36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="29" t="n">
+      <c r="A37" s="27" t="n">
         <v>301</v>
       </c>
-      <c r="B37" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="C37" s="30" t="s">
+      <c r="B37" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="E37" s="29" t="n">
+      <c r="E37" s="27" t="n">
         <v>6</v>
       </c>
-      <c r="F37" s="29" t="s">
+      <c r="F37" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="G37" s="29" t="s">
+      <c r="G37" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="H37" s="17"/>
+      <c r="H37" s="21"/>
       <c r="I37" s="15"/>
-      <c r="J37" s="16"/>
+      <c r="J37" s="2"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
@@ -1954,30 +1948,30 @@
       <c r="V37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="29" t="n">
+      <c r="A38" s="27" t="n">
         <v>302</v>
       </c>
-      <c r="B38" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="C38" s="30" t="s">
+      <c r="B38" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="D38" s="31" t="s">
+      <c r="D38" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="E38" s="29" t="n">
+      <c r="E38" s="27" t="n">
         <v>3</v>
       </c>
-      <c r="F38" s="29" t="s">
+      <c r="F38" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="G38" s="29" t="s">
+      <c r="G38" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="H38" s="17"/>
+      <c r="H38" s="21"/>
       <c r="I38" s="15"/>
-      <c r="J38" s="16"/>
+      <c r="J38" s="2"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
@@ -1992,7 +1986,7 @@
       <c r="V38" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="32" t="s">
+      <c r="D40" s="30" t="s">
         <v>88</v>
       </c>
       <c r="E40" s="0" t="n">

</xml_diff>

<commit_message>
Ajout de la liste des sandwichs + changement dateLivraison en timestamp
</commit_message>
<xml_diff>
--- a/doc/LBS-stories-LP2.xlsx
+++ b/doc/LBS-stories-LP2.xlsx
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="Print_Area_0_0" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Feuille1!$A$1:$G$49</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="90">
   <si>
     <t xml:space="preserve">USER STORIES pour l'application LE BON SANDWICH</t>
   </si>
@@ -219,6 +220,9 @@
   </si>
   <si>
     <t xml:space="preserve">liste des commandes, filtrées sur l'état , triée par date de livraison et ordre de création – permet au point de vente de planifier la préparation des commandes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commandes?statut={statutCommande}</t>
   </si>
   <si>
     <t xml:space="preserve">détail d'une commande</t>
@@ -633,22 +637,22 @@
   </sheetPr>
   <dimension ref="A1:V65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.7040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="22" min="9" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.1632653061225"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="22" min="9" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1489,7 +1493,7 @@
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="38.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11" t="n">
         <v>101</v>
       </c>
@@ -1505,9 +1509,13 @@
       <c r="E25" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="21"/>
+      <c r="F25" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H25" s="14"/>
       <c r="I25" s="15"/>
       <c r="J25" s="2"/>
       <c r="K25" s="3"/>
@@ -1531,10 +1539,10 @@
         <v>1</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E26" s="11" t="n">
         <v>3</v>
@@ -1565,10 +1573,10 @@
         <v>1</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E27" s="11" t="n">
         <v>3</v>
@@ -1593,7 +1601,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B28" s="22"/>
       <c r="C28" s="23"/>
@@ -1663,10 +1671,10 @@
         <v>1</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E30" s="11" t="n">
         <v>5</v>
@@ -1675,7 +1683,7 @@
         <v>38</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H30" s="14"/>
       <c r="I30" s="26"/>
@@ -1701,10 +1709,10 @@
         <v>1</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E31" s="11" t="n">
         <v>5</v>
@@ -1713,7 +1721,7 @@
         <v>38</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H31" s="14"/>
       <c r="I31" s="15"/>
@@ -1739,10 +1747,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E32" s="11" t="n">
         <v>6</v>
@@ -1751,7 +1759,7 @@
         <v>38</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H32" s="21"/>
       <c r="I32" s="15"/>
@@ -1777,10 +1785,10 @@
         <v>3</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E33" s="11" t="n">
         <v>4</v>
@@ -1789,7 +1797,7 @@
         <v>38</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H33" s="14"/>
       <c r="I33" s="15"/>
@@ -1809,7 +1817,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B34" s="22"/>
       <c r="C34" s="23"/>
@@ -1879,19 +1887,19 @@
         <v>1</v>
       </c>
       <c r="C36" s="24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E36" s="11" t="n">
         <v>3</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H36" s="14"/>
       <c r="I36" s="26"/>
@@ -1917,19 +1925,19 @@
         <v>1</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D37" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E37" s="27" t="n">
         <v>6</v>
       </c>
       <c r="F37" s="27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H37" s="21"/>
       <c r="I37" s="15"/>
@@ -1955,19 +1963,19 @@
         <v>1</v>
       </c>
       <c r="C38" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="29" t="s">
         <v>87</v>
-      </c>
-      <c r="D38" s="29" t="s">
-        <v>86</v>
       </c>
       <c r="E38" s="27" t="n">
         <v>3</v>
       </c>
       <c r="F38" s="27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H38" s="21"/>
       <c r="I38" s="15"/>
@@ -1987,7 +1995,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D40" s="30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E40" s="0" t="n">
         <f aca="false">SUM(E7:E38)</f>

</xml_diff>